<commit_message>
19/09/23 - push 1
</commit_message>
<xml_diff>
--- a/sop/aula 6/Pasta1.xlsx
+++ b/sop/aula 6/Pasta1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Guilherme Carvalho\senai\sop\aula 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\senai\sop\aula 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028A87CC-43AB-4A6D-B9E1-02FBFFF3DD57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72DDC44-41FD-4A06-AA7F-E7030C423881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" firstSheet="1" activeTab="7" xr2:uid="{18E1EE1C-A7A3-42D0-8543-3B29665AD687}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{18E1EE1C-A7A3-42D0-8543-3B29665AD687}"/>
   </bookViews>
   <sheets>
     <sheet name="exercício 1" sheetId="1" r:id="rId1"/>
@@ -572,22 +572,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7D81A7-D61A-4CD6-89CC-7A89FC755F9F}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.36328125" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" customWidth="1"/>
-    <col min="5" max="5" width="23.6328125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -617,7 +617,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -629,7 +629,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -641,7 +641,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -653,7 +653,7 @@
         <v>19600</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -678,14 +678,14 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.90625" customWidth="1"/>
-    <col min="2" max="2" width="10.1796875" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -699,7 +699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -714,7 +714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -729,7 +729,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -744,7 +744,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -759,7 +759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -775,7 +775,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D6">
     <sortCondition descending="1" ref="D2"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -790,16 +790,15 @@
       <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" customWidth="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="3" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -816,7 +815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -834,7 +833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -846,7 +845,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -858,7 +857,7 @@
         <v>2140</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -870,7 +869,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -895,13 +894,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -909,7 +908,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -917,7 +916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -925,7 +924,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -933,7 +932,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -941,7 +940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -949,7 +948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -958,7 +957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -980,15 +979,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1002,7 +1001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1017,7 +1016,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1032,7 +1031,7 @@
         <v>74.078150798018711</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1047,7 +1046,7 @@
         <v>59.700283515593355</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1062,7 +1061,7 @@
         <v>68.407186604560209</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1090,14 +1089,14 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" customWidth="1"/>
-    <col min="3" max="3" width="18.90625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -1112,7 +1111,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1139,7 +1138,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -1151,7 +1150,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>7.65</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -1175,7 +1174,7 @@
         <v>5.22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -1187,7 +1186,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1199,7 +1198,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1211,7 +1210,7 @@
         <v>59.4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1223,7 +1222,7 @@
         <v>2.79</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1248,43 +1247,43 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>56464</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>45646</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5464</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4564</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3334</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:A6">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A6">
     <sortCondition descending="1" ref="A2"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1299,13 +1298,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.08984375" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="1" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
@@ -1316,44 +1315,64 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>454</v>
       </c>
       <c r="B2">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <f>A2 + 1/B2</f>
+        <v>454.01785714285717</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>78</v>
       </c>
       <c r="B3">
         <v>345</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <f t="shared" ref="C3:C6" si="0">A3 + 1/B3</f>
+        <v>78.002898550724638</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>24</v>
       </c>
       <c r="B4">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>24.011235955056179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>879</v>
       </c>
       <c r="B5">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>879.02941176470586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>43</v>
       </c>
       <c r="B6">
         <v>67</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>43.014925373134325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>